<commit_message>
same elements array researches has been added
</commit_message>
<xml_diff>
--- a/results/bubble.xlsx
+++ b/results/bubble.xlsx
@@ -1,23 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s\PycharmProjects\sorts\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F661FE9F-EFFF-4A45-B78F-76CEC4F44874}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="straight" sheetId="1" r:id="rId1"/>
     <sheet name="reversed" sheetId="2" r:id="rId2"/>
     <sheet name="sorted" sheetId="3" r:id="rId3"/>
     <sheet name="partly_sorted" sheetId="4" r:id="rId4"/>
+    <sheet name="same_elements" sheetId="5" r:id="rId5"/>
+    <sheet name="partly_same" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="4">
   <si>
     <t>byte</t>
   </si>
@@ -34,8 +42,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +80,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -118,7 +134,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -150,9 +166,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -184,6 +218,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -359,14 +411,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>5</v>
       </c>
@@ -386,7 +438,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -394,13 +446,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.0004072</v>
+        <v>4.0719999999999998E-4</v>
       </c>
       <c r="D2">
-        <v>0.03213339999999999</v>
+        <v>3.2133399999999993E-2</v>
       </c>
       <c r="E2">
-        <v>3.318713</v>
+        <v>3.3187129999999998</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -409,7 +461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -417,10 +469,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0.0003002</v>
+        <v>3.0019999999999998E-4</v>
       </c>
       <c r="D3">
-        <v>0.0395414</v>
+        <v>3.9541399999999997E-2</v>
       </c>
       <c r="E3">
         <v>3.4141016</v>
@@ -432,7 +484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -440,13 +492,13 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0.0003936</v>
+        <v>3.9360000000000003E-4</v>
       </c>
       <c r="D4">
-        <v>0.039949</v>
+        <v>3.9948999999999998E-2</v>
       </c>
       <c r="E4">
-        <v>3.6125116</v>
+        <v>3.6125115999999999</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -455,7 +507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -463,13 +515,13 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0.0004002</v>
+        <v>4.0020000000000002E-4</v>
       </c>
       <c r="D5">
-        <v>0.03423540000000001</v>
+        <v>3.4235400000000013E-2</v>
       </c>
       <c r="E5">
-        <v>3.4773134</v>
+        <v>3.4773133999999999</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -484,14 +536,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>5</v>
       </c>
@@ -511,7 +563,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -519,13 +571,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.0004004000000000001</v>
+        <v>4.0040000000000008E-4</v>
       </c>
       <c r="D2">
-        <v>0.0438042</v>
+        <v>4.3804200000000001E-2</v>
       </c>
       <c r="E2">
-        <v>4.5637956</v>
+        <v>4.5637955999999997</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -534,7 +586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -542,13 +594,13 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0.0006000000000000001</v>
+        <v>6.0000000000000006E-4</v>
       </c>
       <c r="D3">
-        <v>0.0462034</v>
+        <v>4.6203399999999999E-2</v>
       </c>
       <c r="E3">
-        <v>4.9622756</v>
+        <v>4.9622755999999999</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -557,7 +609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -565,13 +617,13 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0.0004002</v>
+        <v>4.0020000000000002E-4</v>
       </c>
       <c r="D4">
-        <v>0.0496048</v>
+        <v>4.9604799999999998E-2</v>
       </c>
       <c r="E4">
-        <v>5.2202856</v>
+        <v>5.2202856000000004</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -580,7 +632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -588,13 +640,13 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0.0005997999999999999</v>
+        <v>5.9979999999999994E-4</v>
       </c>
       <c r="D5">
-        <v>0.04780379999999999</v>
+        <v>4.7803799999999987E-2</v>
       </c>
       <c r="E5">
-        <v>5.231262</v>
+        <v>5.2312620000000001</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -609,14 +661,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>5</v>
       </c>
@@ -636,7 +688,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -650,7 +702,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.0005934</v>
+        <v>5.934E-4</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -659,7 +711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -670,10 +722,10 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.0001994</v>
+        <v>1.994E-4</v>
       </c>
       <c r="E3">
-        <v>0.0006069999999999999</v>
+        <v>6.069999999999999E-4</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -682,7 +734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -696,7 +748,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.0013998</v>
+        <v>1.3998000000000001E-3</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -705,7 +757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -716,10 +768,10 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0.0002002</v>
+        <v>2.0019999999999999E-4</v>
       </c>
       <c r="E5">
-        <v>0.0006002000000000001</v>
+        <v>6.0020000000000006E-4</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -734,14 +786,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>5</v>
       </c>
@@ -761,7 +813,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -769,13 +821,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.0004002</v>
+        <v>4.0020000000000002E-4</v>
       </c>
       <c r="D2">
-        <v>0.0296022</v>
+        <v>2.9602199999999999E-2</v>
       </c>
       <c r="E2">
-        <v>3.2624808</v>
+        <v>3.2624808000000001</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -784,7 +836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -792,10 +844,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0.0003998</v>
+        <v>3.9980000000000001E-4</v>
       </c>
       <c r="D3">
-        <v>0.0335962</v>
+        <v>3.35962E-2</v>
       </c>
       <c r="E3">
         <v>3.469506</v>
@@ -807,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -815,10 +867,10 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0.0002008</v>
+        <v>2.008E-4</v>
       </c>
       <c r="D4">
-        <v>0.03460319999999999</v>
+        <v>3.4603199999999987E-2</v>
       </c>
       <c r="E4">
         <v>4.3021794</v>
@@ -830,7 +882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -838,13 +890,265 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0.0004002</v>
+        <v>4.0020000000000002E-4</v>
       </c>
       <c r="D5">
-        <v>0.0380098</v>
+        <v>3.8009800000000003E-2</v>
       </c>
       <c r="E5">
         <v>3.8673568</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E437EEF-8E85-485C-A3D8-75013AA44595}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>5</v>
+      </c>
+      <c r="C1">
+        <v>50</v>
+      </c>
+      <c r="D1">
+        <v>500</v>
+      </c>
+      <c r="E1">
+        <v>5000</v>
+      </c>
+      <c r="F1">
+        <v>50000</v>
+      </c>
+      <c r="G1">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>5.0100000000000003E-4</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1.0009999999999999E-3</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1.0009999999999999E-3</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0D478A-B562-466C-976C-A17F7B9F8133}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>5</v>
+      </c>
+      <c r="C1">
+        <v>50</v>
+      </c>
+      <c r="D1">
+        <v>500</v>
+      </c>
+      <c r="E1">
+        <v>5000</v>
+      </c>
+      <c r="F1">
+        <v>50000</v>
+      </c>
+      <c r="G1">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>5.0100000000000003E-4</v>
+      </c>
+      <c r="D2">
+        <v>2.8561E-2</v>
+      </c>
+      <c r="E2">
+        <v>3.3049529999999998</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D3">
+        <v>3.1033000000000002E-2</v>
+      </c>
+      <c r="E3">
+        <v>3.6903679999999999</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>3.2534E-2</v>
+      </c>
+      <c r="E4">
+        <v>3.8209919999999999</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>5.0199999999999995E-4</v>
+      </c>
+      <c r="D5">
+        <v>3.0568000000000001E-2</v>
+      </c>
+      <c r="E5">
+        <v>3.6833469999999999</v>
       </c>
       <c r="F5">
         <v>0</v>

</xml_diff>